<commit_message>
heyyooo everything works at Loouis' part
</commit_message>
<xml_diff>
--- a/app/src/main/assets/designlab.xlsx
+++ b/app/src/main/assets/designlab.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projecten\BLEExample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Louis\AndroidStudioProjects\Challenge2\app\src\main\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390"/>
   </bookViews>
   <sheets>
     <sheet name="designlab" sheetId="1" r:id="rId1"/>
@@ -701,24 +701,24 @@
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Berekening" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Controlecel" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Gekoppelde cel" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Goed" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Invoer" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Kop 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Kop 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Kop 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Kop 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Neutraal" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notitie" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Ongeldig" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
-    <cellStyle name="Titel" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Totaal" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Uitvoer" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Verklarende tekst" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Waarschuwingstekst" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -734,9 +734,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -774,7 +774,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -846,7 +846,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -996,18 +996,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>212.5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>88.5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>206.5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>213.5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>190.5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>266.5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>528.5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>602.5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>474.5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>602.5</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>446.5</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>419.5</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>417.5</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>332.5</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>246.5</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>192.5</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>612.5</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>534.5</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>621.5</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>441.5</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>440.5</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>320.5</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>319.5</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>318.5</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>208.5</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>106.5</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>125.5</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>100.5</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>128.5</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>122.5</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>207.5</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>25.5</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>43</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>33.5</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>44</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>337.5</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>430.5</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>531.5</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>618.5</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>543.5</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>585.5</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>431.5</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>51</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>422.5</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>320.5</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>53</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>130.5</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>54</v>
       </c>
@@ -2403,66 +2403,6 @@
       <c r="I50">
         <f t="shared" si="1"/>
         <v>94.5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I52">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I53">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I54">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I55">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I56">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I57">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I58">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I59">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I60">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I61">
-        <f t="shared" si="1"/>
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>